<commit_message>
Added more distances Also, fixed a typo in one of the sheet names
</commit_message>
<xml_diff>
--- a/Documents/Distances.xlsx
+++ b/Documents/Distances.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" tabRatio="752" firstSheet="5" activeTab="13" xr2:uid="{D91A8DBA-E9BB-45E3-84D0-FA2F40E38D3D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" tabRatio="752" firstSheet="11" activeTab="21" xr2:uid="{D91A8DBA-E9BB-45E3-84D0-FA2F40E38D3D}"/>
   </bookViews>
   <sheets>
     <sheet name="From Johnston" sheetId="1" r:id="rId1"/>
     <sheet name="From Robinson" sheetId="2" r:id="rId2"/>
     <sheet name="From the Library" sheetId="3" r:id="rId3"/>
-    <sheet name="From Hendrcks" sheetId="4" r:id="rId4"/>
+    <sheet name="From Hendricks" sheetId="4" r:id="rId4"/>
     <sheet name="From the HUB" sheetId="7" r:id="rId5"/>
     <sheet name="From Lindaman" sheetId="11" r:id="rId6"/>
     <sheet name="From Weyerhaeuser" sheetId="12" r:id="rId7"/>
@@ -3855,7 +3855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0B5204-3871-4413-8844-74B7D13B39BB}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -5156,7 +5156,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5189,20 +5189,24 @@
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="2">
+        <v>826</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1099</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="7" t="str">
+      <c r="H4" s="7">
         <f t="shared" ref="H4:K16" si="0">IF(B4 = "","",(B4/$D$1))</f>
-        <v/>
-      </c>
-      <c r="I4" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>2.1454545454545455</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="0"/>
+        <v>2.8545454545454545</v>
       </c>
       <c r="J4" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5217,16 +5221,18 @@
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>1227</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H5" s="7">
+        <f t="shared" si="0"/>
+        <v>3.1870129870129871</v>
       </c>
       <c r="I5" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5245,20 +5251,24 @@
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="2">
+        <v>640</v>
+      </c>
+      <c r="C6" s="2">
+        <v>732</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="G6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I6" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H6" s="7">
+        <f t="shared" si="0"/>
+        <v>1.6623376623376624</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="0"/>
+        <v>1.9012987012987013</v>
       </c>
       <c r="J6" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5273,16 +5283,18 @@
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>909</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="G7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H7" s="7">
+        <f t="shared" si="0"/>
+        <v>2.361038961038961</v>
       </c>
       <c r="I7" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5301,16 +5313,18 @@
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>840</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="G8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H8" s="7">
+        <f t="shared" si="0"/>
+        <v>2.1818181818181817</v>
       </c>
       <c r="I8" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5357,16 +5371,18 @@
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>1644</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="G10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H10" s="7">
+        <f t="shared" si="0"/>
+        <v>4.2701298701298702</v>
       </c>
       <c r="I10" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5385,16 +5401,18 @@
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>1717</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="G11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
+        <v>4.4597402597402596</v>
       </c>
       <c r="I11" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5413,20 +5431,24 @@
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="2">
+        <v>1674</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1556</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="G12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I12" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H12" s="7">
+        <f t="shared" si="0"/>
+        <v>4.3480519480519479</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="0"/>
+        <v>4.0415584415584416</v>
       </c>
       <c r="J12" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5441,20 +5463,24 @@
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="2">
+        <v>1550</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1750</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="G13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I13" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H13" s="7">
+        <f t="shared" si="0"/>
+        <v>4.0259740259740262</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="0"/>
+        <v>4.5454545454545459</v>
       </c>
       <c r="J13" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5497,16 +5523,18 @@
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>1624</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="G15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H15" s="7">
+        <f t="shared" si="0"/>
+        <v>4.2181818181818178</v>
       </c>
       <c r="I15" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5525,16 +5553,18 @@
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>1916</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="G16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H16" s="7">
+        <f t="shared" si="0"/>
+        <v>4.9766233766233769</v>
       </c>
       <c r="I16" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5560,7 +5590,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5593,20 +5623,24 @@
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="2">
+        <v>1253</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1086</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="7" t="str">
+      <c r="H4" s="7">
         <f t="shared" ref="H4:K16" si="0">IF(B4 = "","",(B4/$D$1))</f>
-        <v/>
-      </c>
-      <c r="I4" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>3.2545454545454544</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="0"/>
+        <v>2.8207792207792206</v>
       </c>
       <c r="J4" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5621,16 +5655,18 @@
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>1157</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H5" s="7">
+        <f t="shared" si="0"/>
+        <v>3.005194805194805</v>
       </c>
       <c r="I5" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5649,16 +5685,18 @@
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>783</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="G6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H6" s="7">
+        <f t="shared" si="0"/>
+        <v>2.0337662337662339</v>
       </c>
       <c r="I6" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5677,16 +5715,18 @@
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>1080</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="G7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H7" s="7">
+        <f t="shared" si="0"/>
+        <v>2.8051948051948052</v>
       </c>
       <c r="I7" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5705,16 +5745,18 @@
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>788</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="G8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H8" s="7">
+        <f t="shared" si="0"/>
+        <v>2.0467532467532465</v>
       </c>
       <c r="I8" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5761,16 +5803,18 @@
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>1565</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="G10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H10" s="7">
+        <f t="shared" si="0"/>
+        <v>4.0649350649350646</v>
       </c>
       <c r="I10" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5789,16 +5833,18 @@
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>1623</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="G11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
+        <v>4.2155844155844155</v>
       </c>
       <c r="I11" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5817,16 +5863,18 @@
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>1498</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="G12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H12" s="7">
+        <f t="shared" si="0"/>
+        <v>3.8909090909090911</v>
       </c>
       <c r="I12" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5845,16 +5893,18 @@
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>1680</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="G13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H13" s="7">
+        <f t="shared" si="0"/>
+        <v>4.3636363636363633</v>
       </c>
       <c r="I13" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5901,16 +5951,18 @@
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>1823</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="G15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H15" s="7">
+        <f t="shared" si="0"/>
+        <v>4.7350649350649352</v>
       </c>
       <c r="I15" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5929,16 +5981,18 @@
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>1890</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="G16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H16" s="7">
+        <f t="shared" si="0"/>
+        <v>4.9090909090909092</v>
       </c>
       <c r="I16" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5964,7 +6018,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5997,20 +6051,24 @@
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="2">
+        <v>916</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1023</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="7" t="str">
+      <c r="H4" s="7">
         <f t="shared" ref="H4:K16" si="0">IF(B4 = "","",(B4/$D$1))</f>
-        <v/>
-      </c>
-      <c r="I4" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>2.3792207792207791</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="0"/>
+        <v>2.657142857142857</v>
       </c>
       <c r="J4" s="7" t="str">
         <f t="shared" si="0"/>
@@ -6025,16 +6083,18 @@
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>946</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H5" s="7">
+        <f t="shared" si="0"/>
+        <v>2.4571428571428573</v>
       </c>
       <c r="I5" s="7" t="str">
         <f t="shared" si="0"/>
@@ -6053,16 +6113,18 @@
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>545</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="G6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H6" s="7">
+        <f t="shared" si="0"/>
+        <v>1.4155844155844155</v>
       </c>
       <c r="I6" s="7" t="str">
         <f t="shared" si="0"/>
@@ -6081,16 +6143,18 @@
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>1125</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="G7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H7" s="7">
+        <f t="shared" si="0"/>
+        <v>2.9220779220779223</v>
       </c>
       <c r="I7" s="7" t="str">
         <f t="shared" si="0"/>
@@ -6109,16 +6173,18 @@
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>551</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="G8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H8" s="7">
+        <f t="shared" si="0"/>
+        <v>1.4311688311688311</v>
       </c>
       <c r="I8" s="7" t="str">
         <f t="shared" si="0"/>
@@ -6165,16 +6231,18 @@
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>1339</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="G10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H10" s="7">
+        <f t="shared" si="0"/>
+        <v>3.4779220779220781</v>
       </c>
       <c r="I10" s="7" t="str">
         <f t="shared" si="0"/>
@@ -6193,16 +6261,18 @@
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>1484</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="G11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
+        <v>3.8545454545454545</v>
       </c>
       <c r="I11" s="7" t="str">
         <f t="shared" si="0"/>
@@ -6221,16 +6291,18 @@
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>1273</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="G12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H12" s="7">
+        <f t="shared" si="0"/>
+        <v>3.3064935064935064</v>
       </c>
       <c r="I12" s="7" t="str">
         <f t="shared" si="0"/>
@@ -6249,16 +6321,18 @@
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>1441</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="G13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H13" s="7">
+        <f t="shared" si="0"/>
+        <v>3.7428571428571429</v>
       </c>
       <c r="I13" s="7" t="str">
         <f t="shared" si="0"/>
@@ -6305,16 +6379,18 @@
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>1769</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="G15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H15" s="7">
+        <f t="shared" si="0"/>
+        <v>4.5948051948051951</v>
       </c>
       <c r="I15" s="7" t="str">
         <f t="shared" si="0"/>
@@ -6333,16 +6409,18 @@
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>1606</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="G16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H16" s="7">
+        <f t="shared" si="0"/>
+        <v>4.1714285714285717</v>
       </c>
       <c r="I16" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7044,7 +7122,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7077,16 +7155,18 @@
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>1142</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="7" t="str">
+      <c r="H4" s="7">
         <f t="shared" ref="H4:K16" si="0">IF(B4 = "","",(B4/$D$1))</f>
-        <v/>
+        <v>2.9662337662337661</v>
       </c>
       <c r="I4" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7105,16 +7185,18 @@
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>548</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H5" s="7">
+        <f t="shared" si="0"/>
+        <v>1.4233766233766234</v>
       </c>
       <c r="I5" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7133,16 +7215,18 @@
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>1015</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="G6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H6" s="7">
+        <f t="shared" si="0"/>
+        <v>2.6363636363636362</v>
       </c>
       <c r="I6" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7161,16 +7245,18 @@
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>728</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="G7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.8909090909090909</v>
       </c>
       <c r="I7" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7189,16 +7275,18 @@
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>885</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="G8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H8" s="7">
+        <f t="shared" si="0"/>
+        <v>2.2987012987012987</v>
       </c>
       <c r="I8" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7245,16 +7333,18 @@
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>509</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="G10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H10" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3220779220779222</v>
       </c>
       <c r="I10" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7273,16 +7363,18 @@
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>310</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="G11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
+        <v>0.80519480519480524</v>
       </c>
       <c r="I11" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7301,20 +7393,24 @@
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="2">
+        <v>622</v>
+      </c>
+      <c r="C12" s="2">
+        <v>684</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="G12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I12" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H12" s="7">
+        <f t="shared" si="0"/>
+        <v>1.6155844155844157</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="0"/>
+        <v>1.7766233766233765</v>
       </c>
       <c r="J12" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7329,16 +7425,18 @@
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>517</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="G13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H13" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3428571428571427</v>
       </c>
       <c r="I13" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7385,16 +7483,18 @@
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>976</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="G15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H15" s="7">
+        <f t="shared" si="0"/>
+        <v>2.535064935064935</v>
       </c>
       <c r="I15" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7413,16 +7513,18 @@
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>593</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="G16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H16" s="7">
+        <f t="shared" si="0"/>
+        <v>1.5402597402597402</v>
       </c>
       <c r="I16" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7448,7 +7550,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7481,20 +7583,24 @@
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="2">
+        <v>916</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1024</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="7" t="str">
+      <c r="H4" s="7">
         <f t="shared" ref="H4:K16" si="0">IF(B4 = "","",(B4/$D$1))</f>
-        <v/>
-      </c>
-      <c r="I4" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>2.3792207792207791</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="0"/>
+        <v>2.6597402597402597</v>
       </c>
       <c r="J4" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7509,16 +7615,18 @@
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>788</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H5" s="7">
+        <f t="shared" si="0"/>
+        <v>2.0467532467532465</v>
       </c>
       <c r="I5" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7537,16 +7645,18 @@
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>939</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="G6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H6" s="7">
+        <f t="shared" si="0"/>
+        <v>2.4389610389610388</v>
       </c>
       <c r="I6" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7565,16 +7675,18 @@
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>590</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="G7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.5324675324675325</v>
       </c>
       <c r="I7" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7593,16 +7705,18 @@
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>1132</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="G8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H8" s="7">
+        <f t="shared" si="0"/>
+        <v>2.9402597402597404</v>
       </c>
       <c r="I8" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7649,16 +7763,18 @@
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>1100</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="G10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H10" s="7">
+        <f t="shared" si="0"/>
+        <v>2.8571428571428572</v>
       </c>
       <c r="I10" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7677,16 +7793,18 @@
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>859</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="G11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
+        <v>2.2311688311688314</v>
       </c>
       <c r="I11" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7705,16 +7823,18 @@
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>487</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="G12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H12" s="7">
+        <f t="shared" si="0"/>
+        <v>1.264935064935065</v>
       </c>
       <c r="I12" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7733,16 +7853,18 @@
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>247</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="G13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.64155844155844155</v>
       </c>
       <c r="I13" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7789,16 +7911,18 @@
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>591</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="G15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H15" s="7">
+        <f t="shared" si="0"/>
+        <v>1.535064935064935</v>
       </c>
       <c r="I15" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7817,16 +7941,18 @@
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>886</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="G16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H16" s="7">
+        <f t="shared" si="0"/>
+        <v>2.3012987012987014</v>
       </c>
       <c r="I16" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7851,8 +7977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D20933CD-FD85-4836-9024-7FF42242AD8E}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7885,20 +8011,24 @@
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="2">
+        <v>1114</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1016</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="7" t="str">
+      <c r="H4" s="7">
         <f t="shared" ref="H4:K16" si="0">IF(B4 = "","",(B4/$D$1))</f>
-        <v/>
-      </c>
-      <c r="I4" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>2.8935064935064934</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="0"/>
+        <v>2.638961038961039</v>
       </c>
       <c r="J4" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7913,16 +8043,18 @@
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>914</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H5" s="7">
+        <f t="shared" si="0"/>
+        <v>2.3740259740259742</v>
       </c>
       <c r="I5" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7941,16 +8073,18 @@
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>1057</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="G6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H6" s="7">
+        <f t="shared" si="0"/>
+        <v>2.7454545454545456</v>
       </c>
       <c r="I6" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7969,16 +8103,18 @@
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>743</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="G7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.92987012987013</v>
       </c>
       <c r="I7" s="7" t="str">
         <f t="shared" si="0"/>
@@ -7997,16 +8133,18 @@
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>1327</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="G8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H8" s="7">
+        <f t="shared" si="0"/>
+        <v>3.4467532467532469</v>
       </c>
       <c r="I8" s="7" t="str">
         <f t="shared" si="0"/>
@@ -8053,16 +8191,18 @@
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>989</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="G10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H10" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5688311688311689</v>
       </c>
       <c r="I10" s="7" t="str">
         <f t="shared" si="0"/>
@@ -8081,16 +8221,18 @@
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>718</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="G11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
+        <v>1.8649350649350649</v>
       </c>
       <c r="I11" s="7" t="str">
         <f t="shared" si="0"/>
@@ -8109,16 +8251,18 @@
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>582</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="G12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H12" s="7">
+        <f t="shared" si="0"/>
+        <v>1.5116883116883117</v>
       </c>
       <c r="I12" s="7" t="str">
         <f t="shared" si="0"/>
@@ -8137,16 +8281,18 @@
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>361</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="G13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.93766233766233764</v>
       </c>
       <c r="I13" s="7" t="str">
         <f t="shared" si="0"/>
@@ -8193,16 +8339,18 @@
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>702</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="G15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H15" s="7">
+        <f t="shared" si="0"/>
+        <v>1.8233766233766233</v>
       </c>
       <c r="I15" s="7" t="str">
         <f t="shared" si="0"/>
@@ -8221,16 +8369,18 @@
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>796</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="G16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H16" s="7">
+        <f t="shared" si="0"/>
+        <v>2.0675324675324673</v>
       </c>
       <c r="I16" s="7" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Forgot to save the spreadsheet before the previous commit
</commit_message>
<xml_diff>
--- a/Documents/Distances.xlsx
+++ b/Documents/Distances.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" tabRatio="752" xr2:uid="{D91A8DBA-E9BB-45E3-84D0-FA2F40E38D3D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" tabRatio="752" firstSheet="11" activeTab="22" xr2:uid="{D91A8DBA-E9BB-45E3-84D0-FA2F40E38D3D}"/>
   </bookViews>
   <sheets>
     <sheet name="From Johnston" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,7 @@
     <sheet name="From Warren" sheetId="22" r:id="rId20"/>
     <sheet name="From Mac" sheetId="23" r:id="rId21"/>
     <sheet name="From Ballard" sheetId="24" r:id="rId22"/>
+    <sheet name="From Facilities" sheetId="25" r:id="rId23"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="69">
   <si>
     <t>Library</t>
   </si>
@@ -246,6 +247,12 @@
   </si>
   <si>
     <t>Times (minutes) from Ballard to…</t>
+  </si>
+  <si>
+    <t>Distances (feet) from Facilities to…</t>
+  </si>
+  <si>
+    <t>Times (minutes) from Facilities to…</t>
   </si>
 </sst>
 </file>
@@ -632,7 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269D6B00-0816-41CA-8210-797105797DE4}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -8429,6 +8436,436 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D298196-5D99-408D-9814-D8109C163955}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="6">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="2">
+        <v>576</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="G4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" ref="H4:K16" si="0">IF(B4 = "","",(B4/$D$1))</f>
+        <v>1.4961038961038962</v>
+      </c>
+      <c r="I4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>837</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="G5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="0"/>
+        <v>2.174025974025974</v>
+      </c>
+      <c r="I5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>777</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="G6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
+        <f t="shared" si="0"/>
+        <v>2.0181818181818181</v>
+      </c>
+      <c r="I6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2">
+        <v>462</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="G7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="I7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1156</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="G8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" si="0"/>
+        <v>3.0025974025974027</v>
+      </c>
+      <c r="I8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1784</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="G9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="7">
+        <f t="shared" si="0"/>
+        <v>4.6337662337662335</v>
+      </c>
+      <c r="I9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1157</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="G10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="0"/>
+        <v>3.005194805194805</v>
+      </c>
+      <c r="I10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1038</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="G11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
+        <v>2.6961038961038959</v>
+      </c>
+      <c r="I11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
+        <v>829</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="G12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" si="0"/>
+        <v>2.1532467532467532</v>
+      </c>
+      <c r="I12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2">
+        <v>750</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="G13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="0"/>
+        <v>1.948051948051948</v>
+      </c>
+      <c r="I13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="2">
+        <v>347</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="G14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.90129870129870127</v>
+      </c>
+      <c r="I14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2">
+        <v>593</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="G15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="7">
+        <f t="shared" si="0"/>
+        <v>1.5402597402597402</v>
+      </c>
+      <c r="I15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1409</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="G16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="7">
+        <f t="shared" si="0"/>
+        <v>3.6597402597402597</v>
+      </c>
+      <c r="I16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42DFD716-EFB0-4289-B6D0-CCC044E8C380}">
   <dimension ref="A1:K24"/>

</xml_diff>